<commit_message>
Carga de Excel, read and write
</commit_message>
<xml_diff>
--- a/app/static/AngularJS/Configurador/FormatoExcelDeUnidades.xlsx
+++ b/app/static/AngularJS/Configurador/FormatoExcelDeUnidades.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Produccion\ASE\ASEv2\app\static\AngularJS\Configurador\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="465" windowWidth="21840" windowHeight="13740" tabRatio="500"/>
   </bookViews>
@@ -19,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>Número Económico</t>
   </si>
@@ -67,6 +72,39 @@
   </si>
   <si>
     <t>16260516-0010</t>
+  </si>
+  <si>
+    <t>placas</t>
+  </si>
+  <si>
+    <t>GFE450</t>
+  </si>
+  <si>
+    <t>GFE451</t>
+  </si>
+  <si>
+    <t>GFE452</t>
+  </si>
+  <si>
+    <t>GFE453</t>
+  </si>
+  <si>
+    <t>GFE454</t>
+  </si>
+  <si>
+    <t>GFE455</t>
+  </si>
+  <si>
+    <t>GFE456</t>
+  </si>
+  <si>
+    <t>GFE457</t>
+  </si>
+  <si>
+    <t>GFE458</t>
+  </si>
+  <si>
+    <t>GFE459</t>
   </si>
 </sst>
 </file>
@@ -141,6 +179,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -401,7 +442,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -412,7 +453,7 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -443,11 +484,13 @@
       <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3"/>
+      <c r="G1" s="3" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
-        <v>1633010407001</v>
+        <v>1163301040735</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>6</v>
@@ -462,12 +505,15 @@
         <v>0</v>
       </c>
       <c r="F2" s="1">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="G2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
-        <v>1633010407002</v>
+        <v>1633010407032</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>7</v>
@@ -482,7 +528,10 @@
         <v>0</v>
       </c>
       <c r="F3" s="1">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="G3" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -502,7 +551,10 @@
         <v>0</v>
       </c>
       <c r="F4" s="1">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="G4" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -522,7 +574,10 @@
         <v>0</v>
       </c>
       <c r="F5" s="1">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="G5" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -542,7 +597,10 @@
         <v>0</v>
       </c>
       <c r="F6" s="1">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="G6" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -562,7 +620,10 @@
         <v>0</v>
       </c>
       <c r="F7" s="1">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="G7" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -582,7 +643,10 @@
         <v>0</v>
       </c>
       <c r="F8" s="1">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="G8" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -602,7 +666,10 @@
         <v>0</v>
       </c>
       <c r="F9" s="1">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="G9" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -622,7 +689,10 @@
         <v>0</v>
       </c>
       <c r="F10" s="1">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="G10" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -642,7 +712,10 @@
         <v>0</v>
       </c>
       <c r="F11" s="1">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="G11" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>